<commit_message>
Answer Report to be tested more
</commit_message>
<xml_diff>
--- a/AnswersReport.xlsx
+++ b/AnswersReport.xlsx
@@ -12,18 +12,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
-  <si>
-    <t>Worker ID</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+  <si>
+    <t>User ID</t>
+  </si>
+  <si>
+    <t>Session ID</t>
   </si>
   <si>
     <t>Orig. ID</t>
   </si>
   <si>
-    <t>I_CANT_TELL</t>
+    <t>dcardos2</t>
+  </si>
+  <si>
+    <t>PROBABLY_NOT</t>
+  </si>
+  <si>
+    <t>sssguy</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>donatella</t>
+  </si>
+  <si>
+    <t>SKIPPED</t>
   </si>
   <si>
     <t>Unanswered</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -75,16 +96,15 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="12.17578125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="7.65234375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="12.53125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="2.0625" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="2.0625" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="2.0625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="10.01171875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="7.65234375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="15.34765625" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="4.16015625" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="8.37109375" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="2.0625" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="2.0625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="2.09765625" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="2.0625" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="2.0625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="2.04296875" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="2.04296875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -94,49 +114,53 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="n">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="n">
         <v>0.0</v>
       </c>
-      <c r="D1" t="n">
+      <c r="E1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G1" t="n">
         <v>9.0</v>
       </c>
-      <c r="E1" t="n">
+      <c r="H1" t="n">
         <v>8.0</v>
       </c>
-      <c r="F1" t="n">
+      <c r="I1" t="n">
         <v>7.0</v>
       </c>
-      <c r="G1" t="n">
+      <c r="J1" t="n">
         <v>6.0</v>
       </c>
-      <c r="H1" t="n">
+      <c r="K1" t="n">
         <v>5.0</v>
       </c>
-      <c r="I1" t="n">
+      <c r="L1" t="n">
         <v>4.0</v>
       </c>
-      <c r="J1" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="K1" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="L1" t="n">
-        <v>1.0</v>
-      </c>
       <c r="M1" t="n">
-        <v>10.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="n">
         <v>0.0</v>
       </c>
-      <c r="B2"/>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2"/>
+      <c r="C2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
       <c r="E2"/>
       <c r="F2"/>
       <c r="G2"/>
@@ -148,15 +172,19 @@
       <c r="M2"/>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="B3"/>
-      <c r="C3" t="s">
-        <v>2</v>
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1.0</v>
       </c>
       <c r="D3"/>
-      <c r="E3"/>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
       <c r="F3"/>
       <c r="G3"/>
       <c r="H3"/>
@@ -168,42 +196,65 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B4" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="C4" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="D4" t="n">
-        <v>9.0</v>
-      </c>
-      <c r="E4" t="n">
-        <v>9.0</v>
-      </c>
-      <c r="F4" t="n">
-        <v>9.0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>9.0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>9.0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>9.0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>9.0</v>
-      </c>
-      <c r="K4" t="n">
-        <v>9.0</v>
-      </c>
-      <c r="L4" t="n">
-        <v>9.0</v>
-      </c>
-      <c r="M4" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D4"/>
+      <c r="E4"/>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
+      <c r="M4"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="M5" t="n">
         <v>3.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Still trying to find the bug
</commit_message>
<xml_diff>
--- a/AnswersReport.xlsx
+++ b/AnswersReport.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>User ID</t>
   </si>
@@ -23,46 +23,43 @@
     <t>Orig. ID</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0ee7e2E-3-83</t>
+  </si>
+  <si>
+    <t>I_CANT_TELL</t>
+  </si>
+  <si>
     <t>2</t>
   </si>
   <si>
-    <t>0Ic-2I-5g-1-5-5</t>
-  </si>
-  <si>
-    <t>I_CANT_TELL</t>
+    <t>1iG-2I5c1-4-9</t>
+  </si>
+  <si>
+    <t>PROBABLY_NOT</t>
   </si>
   <si>
     <t>3</t>
   </si>
   <si>
-    <t>1AA8E-4A-723</t>
-  </si>
-  <si>
-    <t>YES</t>
+    <t>2EI-4i2G-5-2-7</t>
+  </si>
+  <si>
+    <t>NO</t>
   </si>
   <si>
     <t>4</t>
   </si>
   <si>
-    <t>2Gi-3C2e0-1-9</t>
-  </si>
-  <si>
-    <t>NO</t>
+    <t>3gI-3a8g05-8</t>
   </si>
   <si>
     <t>5</t>
   </si>
   <si>
-    <t>3gc1G-3g0-9-1</t>
-  </si>
-  <si>
-    <t>PROBABLY_YES</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>?</t>
+    <t>4Ei0e-6g5-3-1</t>
   </si>
   <si>
     <t>Unanswered</t>
@@ -120,13 +117,13 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="12.17578125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="14.08984375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="14.08984375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="13.8203125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="13.8203125" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="12.53125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="4.16015625" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="15.34765625" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="3.7265625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="14.5546875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="2.07421875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="3.7265625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="12.53125" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="2.0625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="2.0625" customWidth="true" bestFit="true"/>
   </cols>
@@ -142,19 +139,19 @@
         <v>2</v>
       </c>
       <c r="D1" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E1" t="n">
         <v>1.0</v>
       </c>
-      <c r="E1" t="n">
+      <c r="F1" t="n">
         <v>2.0</v>
       </c>
-      <c r="F1" t="n">
+      <c r="G1" t="n">
         <v>3.0</v>
       </c>
-      <c r="G1" t="n">
+      <c r="H1" t="n">
         <v>4.0</v>
-      </c>
-      <c r="H1" t="n">
-        <v>0.0</v>
       </c>
       <c r="I1" t="n">
         <v>9.0</v>
@@ -255,7 +252,7 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H5"/>
       <c r="I5"/>
@@ -266,16 +263,20 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="B6"/>
-      <c r="C6"/>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
       <c r="D6"/>
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6"/>
       <c r="H6" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="I6"/>
       <c r="J6"/>
@@ -285,43 +286,43 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" t="n">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
       <c r="E7" t="n">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
       <c r="F7" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="G7" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="H7" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="I7" t="n">
         <v>3.0</v>
       </c>
       <c r="J7" t="n">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
       <c r="K7" t="n">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
       <c r="L7" t="n">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
       <c r="M7" t="n">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Skill Test bug fixed (but without feature to handle selection)
</commit_message>
<xml_diff>
--- a/AnswersReport.xlsx
+++ b/AnswersReport.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="39">
   <si>
     <t>User ID</t>
   </si>
@@ -26,40 +26,103 @@
     <t>1</t>
   </si>
   <si>
-    <t>0ee7e2E-3-83</t>
+    <t>0II-1i1g0-40</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>1cE-9I6C-15-8</t>
+  </si>
+  <si>
+    <t>SKIPPED</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>2GE7i-1E586</t>
+  </si>
+  <si>
+    <t>PROBABLY_YES</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>3CI0g0a9-75</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>4CI-1i0A8-58</t>
+  </si>
+  <si>
+    <t>PROBABLY_NOT</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>5aE-1i3I3-2-5</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>6aa-5a5c7-43</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>7ic-9G3e-212</t>
   </si>
   <si>
     <t>I_CANT_TELL</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>1iG-2I5c1-4-9</t>
-  </si>
-  <si>
-    <t>PROBABLY_NOT</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>2EI-4i2G-5-2-7</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>3gI-3a8g05-8</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>4Ei0e-6g5-3-1</t>
+    <t>9</t>
+  </si>
+  <si>
+    <t>8Ac-6A-8i9-17</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>9eI2C-2C020</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>10CI-5g-9E41-2</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>32ga8i0G-80-3</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>31ig-6a0E903</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>30GA0e-5E882</t>
   </si>
   <si>
     <t>Unanswered</t>
@@ -117,15 +180,16 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="12.17578125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="13.8203125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="13.8203125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="12.53125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="15.34765625" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="3.7265625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="3.7265625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="12.53125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="2.0625" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="2.0625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="14.51171875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="14.51171875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="8.37109375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="12.53125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="14.5546875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="8.37109375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="15.34765625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="3.7265625" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="4.16015625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="12.53125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -154,19 +218,22 @@
         <v>4.0</v>
       </c>
       <c r="I1" t="n">
-        <v>9.0</v>
+        <v>5.0</v>
       </c>
       <c r="J1" t="n">
-        <v>8.0</v>
+        <v>6.0</v>
       </c>
       <c r="K1" t="n">
         <v>7.0</v>
       </c>
       <c r="L1" t="n">
-        <v>6.0</v>
+        <v>8.0</v>
       </c>
       <c r="M1" t="n">
-        <v>5.0</v>
+        <v>9.0</v>
+      </c>
+      <c r="N1" t="n">
+        <v>10.0</v>
       </c>
     </row>
     <row r="2">
@@ -191,6 +258,7 @@
       <c r="K2"/>
       <c r="L2"/>
       <c r="M2"/>
+      <c r="N2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
@@ -214,6 +282,7 @@
       <c r="K3"/>
       <c r="L3"/>
       <c r="M3"/>
+      <c r="N3"/>
     </row>
     <row r="4">
       <c r="A4" t="s">
@@ -237,6 +306,7 @@
       <c r="K4"/>
       <c r="L4"/>
       <c r="M4"/>
+      <c r="N4"/>
     </row>
     <row r="5">
       <c r="A5" t="s">
@@ -252,7 +322,7 @@
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H5"/>
       <c r="I5"/>
@@ -260,6 +330,7 @@
       <c r="K5"/>
       <c r="L5"/>
       <c r="M5"/>
+      <c r="N5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
@@ -276,53 +347,273 @@
       <c r="F6"/>
       <c r="G6"/>
       <c r="H6" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="I6"/>
       <c r="J6"/>
       <c r="K6"/>
       <c r="L6"/>
       <c r="M6"/>
+      <c r="N6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="E7" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="F7" t="n">
+        <v>18</v>
+      </c>
+      <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9"/>
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9" t="s">
+        <v>24</v>
+      </c>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10" t="s">
+        <v>21</v>
+      </c>
+      <c r="M10"/>
+      <c r="N10"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11"/>
+      <c r="K11"/>
+      <c r="L11"/>
+      <c r="M11" t="s">
+        <v>24</v>
+      </c>
+      <c r="N11"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13"/>
+      <c r="K13"/>
+      <c r="L13"/>
+      <c r="M13"/>
+      <c r="N13"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14"/>
+      <c r="E14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="J14"/>
+      <c r="K14"/>
+      <c r="L14"/>
+      <c r="M14"/>
+      <c r="N14"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15"/>
+      <c r="H15"/>
+      <c r="I15"/>
+      <c r="J15"/>
+      <c r="K15"/>
+      <c r="L15"/>
+      <c r="M15"/>
+      <c r="N15"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G16" t="n">
         <v>4.0</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H16" t="n">
         <v>4.0</v>
       </c>
-      <c r="H7" t="n">
+      <c r="I16" t="n">
         <v>4.0</v>
       </c>
-      <c r="I7" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="J7" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="K7" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="L7" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="M7" t="n">
-        <v>6.0</v>
+      <c r="J16" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="K16" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="L16" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="M16" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="N16" t="n">
+        <v>2.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Fixed answer duplication in reports"
This reverts commit f29abb35643baa1b704a3798c62742ef1fd28e22.
</commit_message>
<xml_diff>
--- a/AnswersReport.xlsx
+++ b/AnswersReport.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="39">
   <si>
     <t>User ID</t>
   </si>
@@ -26,28 +26,103 @@
     <t>1</t>
   </si>
   <si>
-    <t>0ei5I3a764</t>
+    <t>0II-1i1g0-40</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>1cE-9I6C-15-8</t>
+  </si>
+  <si>
+    <t>SKIPPED</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>2GE7i-1E586</t>
   </si>
   <si>
     <t>PROBABLY_YES</t>
   </si>
   <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>3CI0g0a9-75</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>4CI-1i0A8-58</t>
+  </si>
+  <si>
+    <t>PROBABLY_NOT</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>5aE-1i3I3-2-5</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>6aa-5a5c7-43</t>
+  </si>
+  <si>
     <t>YES</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>1CI-1e-8i52-4</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>2Ie5I5C1-5-8</t>
-  </si>
-  <si>
-    <t>SKIPPED</t>
+    <t>8</t>
+  </si>
+  <si>
+    <t>7ic-9G3e-212</t>
+  </si>
+  <si>
+    <t>I_CANT_TELL</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>8Ac-6A-8i9-17</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>9eI2C-2C020</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>10CI-5g-9E41-2</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>32ga8i0G-80-3</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>31ig-6a0E903</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>30GA0e-5E882</t>
   </si>
   <si>
     <t>Unanswered</t>
@@ -105,17 +180,16 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="12.17578125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="12.88671875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="12.88671875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="14.5546875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="4.16015625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="14.51171875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="14.51171875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="8.37109375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="12.53125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="14.5546875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="4.16015625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="8.37109375" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="3.078125" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="3.078125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="2.0625" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" width="2.0625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="8.37109375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="15.34765625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="3.7265625" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="4.16015625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="12.53125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -132,10 +206,10 @@
         <v>0.0</v>
       </c>
       <c r="E1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F1" t="n">
         <v>2.0</v>
-      </c>
-      <c r="F1" t="n">
-        <v>1.0</v>
       </c>
       <c r="G1" t="n">
         <v>3.0</v>
@@ -144,25 +218,22 @@
         <v>4.0</v>
       </c>
       <c r="I1" t="n">
-        <v>11.0</v>
+        <v>5.0</v>
       </c>
       <c r="J1" t="n">
-        <v>10.0</v>
+        <v>6.0</v>
       </c>
       <c r="K1" t="n">
-        <v>9.0</v>
+        <v>7.0</v>
       </c>
       <c r="L1" t="n">
         <v>8.0</v>
       </c>
       <c r="M1" t="n">
-        <v>7.0</v>
+        <v>9.0</v>
       </c>
       <c r="N1" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="O1" t="n">
-        <v>5.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="2">
@@ -178,9 +249,7 @@
       <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
+      <c r="E2"/>
       <c r="F2"/>
       <c r="G2"/>
       <c r="H2"/>
@@ -190,26 +259,23 @@
       <c r="L2"/>
       <c r="M2"/>
       <c r="N2"/>
-      <c r="O2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3"/>
+      <c r="E3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" t="s">
-        <v>6</v>
-      </c>
+      <c r="F3"/>
+      <c r="G3"/>
       <c r="H3"/>
       <c r="I3"/>
       <c r="J3"/>
@@ -217,7 +283,6 @@
       <c r="L3"/>
       <c r="M3"/>
       <c r="N3"/>
-      <c r="O3"/>
     </row>
     <row r="4">
       <c r="A4" t="s">
@@ -231,18 +296,17 @@
       </c>
       <c r="D4"/>
       <c r="E4"/>
-      <c r="F4"/>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
       <c r="G4"/>
-      <c r="H4" t="s">
-        <v>11</v>
-      </c>
+      <c r="H4"/>
       <c r="I4"/>
       <c r="J4"/>
       <c r="K4"/>
       <c r="L4"/>
       <c r="M4"/>
       <c r="N4"/>
-      <c r="O4"/>
     </row>
     <row r="5">
       <c r="A5" t="s">
@@ -254,41 +318,302 @@
       <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5"/>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6"/>
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6"/>
+      <c r="J6"/>
+      <c r="K6"/>
+      <c r="L6"/>
+      <c r="M6"/>
+      <c r="N6"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9"/>
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9" t="s">
+        <v>24</v>
+      </c>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10" t="s">
+        <v>21</v>
+      </c>
+      <c r="M10"/>
+      <c r="N10"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11"/>
+      <c r="K11"/>
+      <c r="L11"/>
+      <c r="M11" t="s">
+        <v>24</v>
+      </c>
+      <c r="N11"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13"/>
+      <c r="K13"/>
+      <c r="L13"/>
+      <c r="M13"/>
+      <c r="N13"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14"/>
+      <c r="E14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="J14"/>
+      <c r="K14"/>
+      <c r="L14"/>
+      <c r="M14"/>
+      <c r="N14"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15"/>
+      <c r="H15"/>
+      <c r="I15"/>
+      <c r="J15"/>
+      <c r="K15"/>
+      <c r="L15"/>
+      <c r="M15"/>
+      <c r="N15"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F16" t="n">
         <v>2.0</v>
       </c>
-      <c r="E5" t="n">
+      <c r="G16" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="J16" t="n">
         <v>2.0</v>
       </c>
-      <c r="F5" t="n">
+      <c r="K16" t="n">
         <v>2.0</v>
       </c>
-      <c r="G5" t="n">
+      <c r="L16" t="n">
         <v>2.0</v>
       </c>
-      <c r="H5" t="n">
+      <c r="M16" t="n">
         <v>2.0</v>
       </c>
-      <c r="I5" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="J5" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="K5" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="L5" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="M5" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="N5" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="O5" t="n">
-        <v>3.0</v>
+      <c r="N16" t="n">
+        <v>2.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>